<commit_message>
Update shift booking logic and /mybookings command
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\ShiftBookExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\School\SIT_Event\SIT_ProjectHub\ShiftBookExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C0E983-1C3A-41FC-98D2-89EBD5ED4316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DF668E-D3C7-4B3B-9926-CB20D6BC2B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="0" windowWidth="12070" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="630" yWindow="0" windowWidth="12150" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,143 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+  <si>
+    <t>studentID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>nightShift</t>
+  </si>
+  <si>
+    <t>isAdmin</t>
+  </si>
+  <si>
+    <t>specialUser</t>
+  </si>
+  <si>
+    <t>ALEXI KIZHAKKEPURATHU GEORGE</t>
+  </si>
+  <si>
+    <t>CHONG KAI LIN</t>
+  </si>
+  <si>
+    <t>ISAAC SOLOMON WONG</t>
+  </si>
+  <si>
+    <t>RYAN TAN YONG SOON TAN</t>
+  </si>
+  <si>
+    <t>VIC GERSUN MONTANO PAMPLONA</t>
+  </si>
+  <si>
+    <t>WANG CONGYING</t>
+  </si>
+  <si>
+    <t>AKMAL RUSYAIDI BIN MUHAMMAD TAJWID</t>
+  </si>
+  <si>
+    <t>ALICIA WONG YUAN QI</t>
+  </si>
+  <si>
+    <t>BECKHAM BENNY ROSS</t>
+  </si>
+  <si>
+    <t>BENJAMIN LAU REY JUN</t>
+  </si>
+  <si>
+    <t>CALWIN ANG WEI XUAN</t>
+  </si>
+  <si>
+    <t>CELEST GOH ZI XUAN</t>
+  </si>
+  <si>
+    <t>GERALD GOH XUAN CHEE</t>
+  </si>
+  <si>
+    <t>HO ZHI XIAN</t>
+  </si>
+  <si>
+    <t>JEREMIAH HE SHUO</t>
+  </si>
+  <si>
+    <t>JIN ZIYU</t>
+  </si>
+  <si>
+    <t>KOK PING XIAN</t>
+  </si>
+  <si>
+    <t>LEK CHEN PING</t>
+  </si>
+  <si>
+    <t>LEK ER XUN</t>
+  </si>
+  <si>
+    <t>LENG HONGJIE, EVANDER</t>
+  </si>
+  <si>
+    <t>LIM KUN YAO, KEGAN</t>
+  </si>
+  <si>
+    <t>LUKAS TAN LI ZHI</t>
+  </si>
+  <si>
+    <t>MOHAMMAD HAFIZ BIN MOHAMMAD EFFENDI</t>
+  </si>
+  <si>
+    <t>NASHA AFRINA BINTE ABDUL MUTALIB</t>
+  </si>
+  <si>
+    <t>NG JI YIN SAMUEL</t>
+  </si>
+  <si>
+    <t>NG YUEN TAO</t>
+  </si>
+  <si>
+    <t>NUR ALISYA RUSLI</t>
+  </si>
+  <si>
+    <t>PIERRE LIM KIA EN</t>
+  </si>
+  <si>
+    <t>PNG SWEE HIANG</t>
+  </si>
+  <si>
+    <t>RANDY CHONG JUN ER</t>
+  </si>
+  <si>
+    <t>SIM YEE HUI JAMIE</t>
+  </si>
+  <si>
+    <t>STAFFORD HO SHENG XIAN</t>
+  </si>
+  <si>
+    <t>TANG RUI FENG REAGAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THEODOSIUS CHIN GUOJUN </t>
+  </si>
+  <si>
+    <t>TIMOTHY JAMES LIM</t>
+  </si>
+  <si>
+    <t>GALVIN YAP MIN JN</t>
+  </si>
+  <si>
+    <t>YU HAOTONG</t>
+  </si>
+  <si>
+    <t>MUHAMMED IRFAN BIN SHAFARUDIN BIN SHAFARUDIN</t>
+  </si>
+  <si>
+    <t>JESSICA CHOY ING</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,14 +477,818 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3 D5:D6 D8:D11 D14:D17 D19 D21:D22 D24:D26 D31:D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2200950</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>98313994</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2400788</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>81390271</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2401356</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>86604500</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2400867</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>92738285</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2301322</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>85087158</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2400892</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>82651219</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>2303213</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>96667642</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2200116</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>96453543</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>2400766</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>85334319</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>2202029</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>98906662</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2402273</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>82018026</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2400702</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>90034548</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2403380</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>96653059</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2402119</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15">
+        <v>80542572</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2401202</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16">
+        <v>81146752</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2402042</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>96623126</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2003284</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>96543195</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2302643</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19">
+        <v>90062896</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2302801</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>94665118</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2302768</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21">
+        <v>98596867</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2303239</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>88345209</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2302643</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23">
+        <v>90188967</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2400971</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24">
+        <v>87258115</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2402351</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25">
+        <v>83284574</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>2301241</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>92269244</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>2401910</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>86918652</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>2302741</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>97279193</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2303361</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>91123602</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2201218</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>85060453</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>2301350</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31">
+        <v>91736001</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>2102399</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32">
+        <v>80629895</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>2201049</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33">
+        <v>82225191</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>2401574</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34">
+        <v>88663960</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>2302705</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35">
+        <v>88269549</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2401554</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>92477805</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2301451</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>93709168</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>2401236</v>
+      </c>
+      <c r="B38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38">
+        <v>87821022</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>2402492</v>
+      </c>
+      <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39">
+        <v>86127900</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>2402043</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>83228165</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Overwrite with local version
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\School\SIT_Event\SIT_ProjectHub\ShiftBookExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DF668E-D3C7-4B3B-9926-CB20D6BC2B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9317D503-BE01-49CB-841B-BDEDF4EEF088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="0" windowWidth="12150" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,12 +57,6 @@
     <t>RYAN TAN YONG SOON TAN</t>
   </si>
   <si>
-    <t>VIC GERSUN MONTANO PAMPLONA</t>
-  </si>
-  <si>
-    <t>WANG CONGYING</t>
-  </si>
-  <si>
     <t>AKMAL RUSYAIDI BIN MUHAMMAD TAJWID</t>
   </si>
   <si>
@@ -156,10 +150,16 @@
     <t>YU HAOTONG</t>
   </si>
   <si>
-    <t>MUHAMMED IRFAN BIN SHAFARUDIN BIN SHAFARUDIN</t>
-  </si>
-  <si>
-    <t>JESSICA CHOY ING</t>
+    <t>congying</t>
+  </si>
+  <si>
+    <t>irfan</t>
+  </si>
+  <si>
+    <t>jessica</t>
+  </si>
+  <si>
+    <t>vic</t>
   </si>
 </sst>
 </file>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3 D5:D6 D8:D11 D14:D17 D19 D21:D22 D24:D26 D31:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,7 +513,7 @@
         <v>2200950</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>98313994</v>
@@ -553,7 +553,7 @@
         <v>2401356</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>86604500</v>
@@ -573,7 +573,7 @@
         <v>2400867</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>92738285</v>
@@ -593,7 +593,7 @@
         <v>2301322</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>85087158</v>
@@ -613,7 +613,7 @@
         <v>2400892</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>82651219</v>
@@ -633,7 +633,7 @@
         <v>2303213</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>96667642</v>
@@ -673,7 +673,7 @@
         <v>2400766</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>85334319</v>
@@ -693,7 +693,7 @@
         <v>2202029</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>98906662</v>
@@ -733,7 +733,7 @@
         <v>2400702</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>90034548</v>
@@ -753,7 +753,7 @@
         <v>2403380</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>96653059</v>
@@ -773,7 +773,7 @@
         <v>2402119</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>80542572</v>
@@ -793,7 +793,7 @@
         <v>2401202</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>81146752</v>
@@ -813,7 +813,7 @@
         <v>2402042</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>96623126</v>
@@ -833,7 +833,7 @@
         <v>2003284</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>96543195</v>
@@ -853,7 +853,7 @@
         <v>2302643</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>90062896</v>
@@ -873,7 +873,7 @@
         <v>2302801</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>94665118</v>
@@ -893,7 +893,7 @@
         <v>2302768</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>98596867</v>
@@ -913,7 +913,7 @@
         <v>2303239</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>88345209</v>
@@ -933,7 +933,7 @@
         <v>2302643</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>90188967</v>
@@ -953,7 +953,7 @@
         <v>2400971</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <v>87258115</v>
@@ -973,7 +973,7 @@
         <v>2402351</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>83284574</v>
@@ -993,7 +993,7 @@
         <v>2301241</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>92269244</v>
@@ -1013,7 +1013,7 @@
         <v>2401910</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>86918652</v>
@@ -1033,7 +1033,7 @@
         <v>2302741</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>97279193</v>
@@ -1053,7 +1053,7 @@
         <v>2303361</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>91123602</v>
@@ -1073,7 +1073,7 @@
         <v>2201218</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30">
         <v>85060453</v>
@@ -1093,7 +1093,7 @@
         <v>2301350</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>91736001</v>
@@ -1113,7 +1113,7 @@
         <v>2102399</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>80629895</v>
@@ -1133,7 +1133,7 @@
         <v>2201049</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33">
         <v>82225191</v>
@@ -1153,7 +1153,7 @@
         <v>2401574</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>88663960</v>
@@ -1173,7 +1173,7 @@
         <v>2302705</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>88269549</v>
@@ -1213,7 +1213,7 @@
         <v>2301451</v>
       </c>
       <c r="B37" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C37">
         <v>93709168</v>
@@ -1233,7 +1233,7 @@
         <v>2401236</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C38">
         <v>87821022</v>
@@ -1253,7 +1253,7 @@
         <v>2402492</v>
       </c>
       <c r="B39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>86127900</v>
@@ -1273,7 +1273,7 @@
         <v>2402043</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C40">
         <v>83228165</v>

</xml_diff>